<commit_message>
Additionally ,I have posted graph in this.
</commit_message>
<xml_diff>
--- a/Daily Rituals.xlsx
+++ b/Daily Rituals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaba\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DD71C9-D1B9-4A94-BD18-D6F2F357F9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{6819E0D9-C28D-1F4B-9835-BF20D8DF6523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19140" yWindow="1848" windowWidth="7500" windowHeight="6000" activeTab="3" xr2:uid="{EF2822AE-C848-4201-BDBB-D23B423D840F}"/>
   </bookViews>
@@ -18,17 +18,25 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>Charles Darwin</t>
   </si>
@@ -286,6 +294,21 @@
   </si>
   <si>
     <t>cocktail hour &amp; social life + dinner with wine</t>
+  </si>
+  <si>
+    <t>Personalities</t>
+  </si>
+  <si>
+    <t>Time( sleep)</t>
+  </si>
+  <si>
+    <t>Time( Food)</t>
+  </si>
+  <si>
+    <t>Ludwig Van Beethoven</t>
+  </si>
+  <si>
+    <t>WH Auden</t>
   </si>
 </sst>
 </file>
@@ -357,6 +380,1015 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time( sleep)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Benjamin Franklin</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Charles Darwin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Charles Dickens</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sigmund Freud</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Immanuel Kant</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ludwig Van Beethoven</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WH Auden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$10:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0633-2147-B264-DA8618E4B09A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time( Food)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Benjamin Franklin</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Charles Darwin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Charles Dickens</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sigmund Freud</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Immanuel Kant</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ludwig Van Beethoven</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WH Auden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$C$10:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0633-2147-B264-DA8618E4B09A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="666641024"/>
+        <c:axId val="673428864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="666641024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="673428864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="673428864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666641024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>108585</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D79B7A41-5AA7-DC4E-810C-C36DDEA2CDF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -662,15 +1694,15 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.27734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.4765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.46875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.51171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -680,7 +1712,7 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -694,7 +1726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="41.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -708,7 +1740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -722,7 +1754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -736,7 +1768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -750,7 +1782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="27.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -764,7 +1796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -772,7 +1804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -780,7 +1812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -788,7 +1820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -796,7 +1828,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -821,15 +1853,15 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.2578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>53</v>
       </c>
@@ -839,7 +1871,7 @@
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -853,7 +1885,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>0.33333333333333331</v>
       </c>
@@ -867,7 +1899,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -881,7 +1913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -895,7 +1927,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -909,7 +1941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="27.75" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>48</v>
       </c>
@@ -917,7 +1949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>50</v>
       </c>
@@ -942,14 +1974,14 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.56640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.37890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.62109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -959,7 +1991,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -973,7 +2005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -987,7 +2019,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1001,7 +2033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1015,7 +2047,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1029,7 +2061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1037,7 +2069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1045,7 +2077,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1064,23 +2096,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A205AED-AA08-4E46-8D6E-5F49CCA158C5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A9" sqref="A9:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1088,7 +2120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1096,7 +2128,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1104,7 +2136,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -1112,7 +2144,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -1120,7 +2152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1128,7 +2160,96 @@
         <v>85</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>